<commit_message>
switched on active layer + litter layer
</commit_message>
<xml_diff>
--- a/specieslist.xlsx
+++ b/specieslist.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="specieslist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>number</t>
   </si>
@@ -175,12 +175,36 @@
   </si>
   <si>
     <t>rootingdepth</t>
+  </si>
+  <si>
+    <t>minsoilwater</t>
+  </si>
+  <si>
+    <t>biomassleafbase</t>
+  </si>
+  <si>
+    <t>biomassleaffaca</t>
+  </si>
+  <si>
+    <t>biomassleaffacb</t>
+  </si>
+  <si>
+    <t>biomasswoodbase</t>
+  </si>
+  <si>
+    <t>biomasswoodfaca</t>
+  </si>
+  <si>
+    <t>biomasswoodfacb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -658,8 +682,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -981,65 +1008,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU6"/>
+  <dimension ref="A1:BB64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AO2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ13" sqref="AQ13"/>
+      <selection pane="bottomRight" activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.109375" customWidth="1"/>
+    <col min="45" max="45" width="14.88671875" customWidth="1"/>
+    <col min="46" max="46" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1170,19 +1198,40 @@
         <v>47</v>
       </c>
       <c r="AR1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS1" t="s">
         <v>48</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>51</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>49</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>50</v>
       </c>
+      <c r="AW1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1259,16 +1308,16 @@
         <v>8.1878499999999992</v>
       </c>
       <c r="Z2">
-        <v>0.76285499999999995</v>
+        <v>0.4</v>
       </c>
       <c r="AA2">
         <v>0.79295000000000004</v>
       </c>
       <c r="AB2">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AC2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -1289,7 +1338,7 @@
         <v>0.55803000000000003</v>
       </c>
       <c r="AJ2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK2">
         <v>-45</v>
@@ -1310,22 +1359,43 @@
         <v>0.17710000000000001</v>
       </c>
       <c r="AQ2">
+        <v>20</v>
+      </c>
+      <c r="AR2">
+        <v>21.1</v>
+      </c>
+      <c r="AS2">
+        <v>40</v>
+      </c>
+      <c r="AT2">
         <v>50</v>
       </c>
-      <c r="AR2">
-        <v>90</v>
-      </c>
-      <c r="AS2">
-        <v>50</v>
-      </c>
-      <c r="AT2">
+      <c r="AU2">
         <v>2</v>
       </c>
-      <c r="AU2">
+      <c r="AV2">
         <v>0.01</v>
       </c>
+      <c r="AW2">
+        <v>703.62070000000006</v>
+      </c>
+      <c r="AX2" s="1">
+        <v>579.49980000000005</v>
+      </c>
+      <c r="AY2" s="1">
+        <v>208.68700000000001</v>
+      </c>
+      <c r="AZ2">
+        <v>78713.626749999996</v>
+      </c>
+      <c r="BA2">
+        <v>793.64156000000003</v>
+      </c>
+      <c r="BB2">
+        <v>73.913020000000003</v>
+      </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1432,7 +1502,7 @@
         <v>0.55803000000000003</v>
       </c>
       <c r="AJ3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AK3">
         <v>-33</v>
@@ -1456,19 +1526,40 @@
         <v>200</v>
       </c>
       <c r="AR3">
+        <v>10</v>
+      </c>
+      <c r="AS3">
         <v>90</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>100</v>
       </c>
-      <c r="AT3">
+      <c r="AU3">
         <v>2</v>
       </c>
-      <c r="AU3">
+      <c r="AV3">
         <v>0</v>
       </c>
+      <c r="AW3">
+        <v>703.62070000000006</v>
+      </c>
+      <c r="AX3" s="1">
+        <v>579.49980000000005</v>
+      </c>
+      <c r="AY3" s="1">
+        <v>208.68700000000001</v>
+      </c>
+      <c r="AZ3">
+        <v>78713.626749999996</v>
+      </c>
+      <c r="BA3">
+        <v>793.64156000000003</v>
+      </c>
+      <c r="BB3">
+        <v>73.913020000000003</v>
+      </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1599,19 +1690,40 @@
         <v>20</v>
       </c>
       <c r="AR4">
+        <v>10</v>
+      </c>
+      <c r="AS4">
         <v>90</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>20</v>
       </c>
-      <c r="AT4">
+      <c r="AU4">
         <v>2</v>
       </c>
-      <c r="AU4">
+      <c r="AV4">
         <v>0.01</v>
       </c>
+      <c r="AW4" s="2">
+        <v>703.62070000000006</v>
+      </c>
+      <c r="AX4" s="3">
+        <v>579.49980000000005</v>
+      </c>
+      <c r="AY4" s="3">
+        <v>208.68700000000001</v>
+      </c>
+      <c r="AZ4" s="2">
+        <v>78713.626749999996</v>
+      </c>
+      <c r="BA4" s="2">
+        <v>793.64156000000003</v>
+      </c>
+      <c r="BB4" s="2">
+        <v>73.913020000000003</v>
+      </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1742,19 +1854,40 @@
         <v>200</v>
       </c>
       <c r="AR5">
+        <v>10</v>
+      </c>
+      <c r="AS5">
         <v>50</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>200</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>1.5</v>
       </c>
-      <c r="AU5">
+      <c r="AV5">
         <v>0</v>
       </c>
+      <c r="AW5">
+        <v>703.62070000000006</v>
+      </c>
+      <c r="AX5" s="1">
+        <v>579.49980000000005</v>
+      </c>
+      <c r="AY5" s="1">
+        <v>208.68700000000001</v>
+      </c>
+      <c r="AZ5">
+        <v>78713.626749999996</v>
+      </c>
+      <c r="BA5">
+        <v>793.64156000000003</v>
+      </c>
+      <c r="BB5">
+        <v>73.913020000000003</v>
+      </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1885,19 +2018,67 @@
         <v>100</v>
       </c>
       <c r="AR6">
+        <v>10</v>
+      </c>
+      <c r="AS6">
         <v>20</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>100</v>
       </c>
-      <c r="AT6">
+      <c r="AU6">
         <v>3</v>
       </c>
-      <c r="AU6">
+      <c r="AV6">
         <v>0</v>
       </c>
+      <c r="AW6">
+        <v>703.62070000000006</v>
+      </c>
+      <c r="AX6" s="1">
+        <v>579.49980000000005</v>
+      </c>
+      <c r="AY6" s="1">
+        <v>208.68700000000001</v>
+      </c>
+      <c r="AZ6">
+        <v>78713.626749999996</v>
+      </c>
+      <c r="BA6">
+        <v>793.64156000000003</v>
+      </c>
+      <c r="BB6">
+        <v>73.913020000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="39:43" x14ac:dyDescent="0.3">
+      <c r="AO59" s="2"/>
+    </row>
+    <row r="60" spans="39:43" x14ac:dyDescent="0.3">
+      <c r="AM60" s="1"/>
+      <c r="AN60" s="1"/>
+      <c r="AO60" s="3"/>
+      <c r="AP60" s="1"/>
+      <c r="AQ60" s="1"/>
+    </row>
+    <row r="61" spans="39:43" x14ac:dyDescent="0.3">
+      <c r="AM61" s="1"/>
+      <c r="AN61" s="1"/>
+      <c r="AO61" s="3"/>
+      <c r="AP61" s="1"/>
+      <c r="AQ61" s="1"/>
+    </row>
+    <row r="62" spans="39:43" x14ac:dyDescent="0.3">
+      <c r="AO62" s="2"/>
+    </row>
+    <row r="63" spans="39:43" x14ac:dyDescent="0.3">
+      <c r="AO63" s="2"/>
+    </row>
+    <row r="64" spans="39:43" x14ac:dyDescent="0.3">
+      <c r="AO64" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated growth and height allometry; corrected setting cone height
</commit_message>
<xml_diff>
--- a/specieslist.xlsx
+++ b/specieslist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>number</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>biomasswoodfacb</t>
+  </si>
+  <si>
+    <t>heightloga</t>
+  </si>
+  <si>
+    <t>heightlogb</t>
+  </si>
+  <si>
+    <t>heightlogc</t>
   </si>
 </sst>
 </file>
@@ -1008,66 +1017,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB64"/>
+  <dimension ref="A1:BE64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB3" sqref="AB3"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="23.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.109375" customWidth="1"/>
-    <col min="45" max="45" width="14.88671875" customWidth="1"/>
-    <col min="46" max="46" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.140625" customWidth="1"/>
+    <col min="48" max="48" width="14.85546875" customWidth="1"/>
+    <col min="49" max="49" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1135,103 +1147,112 @@
         <v>20</v>
       </c>
       <c r="W1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>47</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>52</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>48</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>51</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>49</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>50</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>53</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>54</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>55</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>56</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>57</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BE1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1263,22 +1284,22 @@
         <v>0.44797500000000001</v>
       </c>
       <c r="K2">
-        <v>-3.0000000000000001E-3</v>
+        <v>-1.331944E-4</v>
       </c>
       <c r="L2">
-        <v>0.03</v>
+        <v>1.4706535999999999E-3</v>
       </c>
       <c r="M2">
-        <v>-1.98</v>
+        <v>-0.80558140430000003</v>
       </c>
       <c r="N2">
-        <v>-3.0000000000000001E-3</v>
+        <v>-1.331944E-4</v>
       </c>
       <c r="O2">
-        <v>0.03</v>
+        <v>1.4706535999999999E-3</v>
       </c>
       <c r="P2">
-        <v>-1.98</v>
+        <v>-0.80558140430000003</v>
       </c>
       <c r="Q2">
         <v>42.88</v>
@@ -1299,103 +1320,112 @@
         <v>7.02</v>
       </c>
       <c r="W2">
+        <v>9.4149999999999991</v>
+      </c>
+      <c r="X2">
+        <v>2.83</v>
+      </c>
+      <c r="Y2">
+        <v>2.214</v>
+      </c>
+      <c r="Z2">
         <v>1E-4</v>
       </c>
-      <c r="X2">
+      <c r="AA2">
         <v>609</v>
       </c>
-      <c r="Y2">
+      <c r="AB2">
         <v>8.1878499999999992</v>
       </c>
-      <c r="Z2">
+      <c r="AC2">
         <v>0.4</v>
       </c>
-      <c r="AA2">
+      <c r="AD2">
         <v>0.79295000000000004</v>
       </c>
-      <c r="AB2">
+      <c r="AE2">
         <v>0.01</v>
       </c>
-      <c r="AC2">
+      <c r="AF2">
         <v>0.1</v>
       </c>
-      <c r="AD2">
+      <c r="AG2">
         <v>0</v>
       </c>
-      <c r="AE2">
+      <c r="AH2">
         <v>0.1</v>
       </c>
-      <c r="AF2">
+      <c r="AI2">
         <v>0.2</v>
       </c>
-      <c r="AG2">
+      <c r="AJ2">
         <v>0.23780499999999999</v>
       </c>
-      <c r="AH2">
+      <c r="AK2">
         <v>0.44724000000000003</v>
       </c>
-      <c r="AI2">
+      <c r="AL2">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AJ2">
+      <c r="AM2">
         <v>4</v>
       </c>
-      <c r="AK2">
+      <c r="AN2">
         <v>-45</v>
       </c>
-      <c r="AL2">
+      <c r="AO2">
         <v>9</v>
       </c>
-      <c r="AM2">
+      <c r="AP2">
         <v>7.8E-2</v>
       </c>
-      <c r="AN2">
+      <c r="AQ2">
         <v>14.824999999999999</v>
       </c>
-      <c r="AO2">
+      <c r="AR2">
         <v>0.108</v>
       </c>
-      <c r="AP2">
+      <c r="AS2">
         <v>0.17710000000000001</v>
       </c>
-      <c r="AQ2">
+      <c r="AT2">
         <v>20</v>
       </c>
-      <c r="AR2">
+      <c r="AU2">
         <v>21.1</v>
       </c>
-      <c r="AS2">
+      <c r="AV2">
         <v>40</v>
       </c>
-      <c r="AT2">
+      <c r="AW2">
         <v>50</v>
       </c>
-      <c r="AU2">
+      <c r="AX2">
         <v>2</v>
       </c>
-      <c r="AV2">
+      <c r="AY2">
         <v>0.01</v>
       </c>
-      <c r="AW2">
+      <c r="AZ2">
         <v>703.62070000000006</v>
       </c>
-      <c r="AX2" s="1">
+      <c r="BA2" s="1">
         <v>579.49980000000005</v>
       </c>
-      <c r="AY2" s="1">
+      <c r="BB2" s="1">
         <v>208.68700000000001</v>
       </c>
-      <c r="AZ2">
+      <c r="BC2">
         <v>78713.626749999996</v>
       </c>
-      <c r="BA2">
+      <c r="BD2">
         <v>793.64156000000003</v>
       </c>
-      <c r="BB2">
+      <c r="BE2">
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1463,103 +1493,112 @@
         <v>7.02</v>
       </c>
       <c r="W3">
+        <v>9.4149999999999991</v>
+      </c>
+      <c r="X3">
+        <v>2.83</v>
+      </c>
+      <c r="Y3">
+        <v>2.214</v>
+      </c>
+      <c r="Z3">
         <v>1E-4</v>
       </c>
-      <c r="X3">
+      <c r="AA3">
         <v>500</v>
       </c>
-      <c r="Y3">
+      <c r="AB3">
         <v>8.1878499999999992</v>
       </c>
-      <c r="Z3">
+      <c r="AC3">
         <v>0.76285499999999995</v>
       </c>
-      <c r="AA3">
+      <c r="AD3">
         <v>0.79295000000000004</v>
       </c>
-      <c r="AB3">
+      <c r="AE3">
         <v>0</v>
       </c>
-      <c r="AC3">
+      <c r="AF3">
         <v>0.5</v>
       </c>
-      <c r="AD3">
+      <c r="AG3">
         <v>0</v>
       </c>
-      <c r="AE3">
+      <c r="AH3">
         <v>0.1</v>
       </c>
-      <c r="AF3">
+      <c r="AI3">
         <v>0.2</v>
       </c>
-      <c r="AG3">
+      <c r="AJ3">
         <v>0.23780499999999999</v>
       </c>
-      <c r="AH3">
+      <c r="AK3">
         <v>0.44724000000000003</v>
       </c>
-      <c r="AI3">
+      <c r="AL3">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AJ3">
+      <c r="AM3">
         <v>1</v>
       </c>
-      <c r="AK3">
+      <c r="AN3">
         <v>-33</v>
       </c>
-      <c r="AL3">
+      <c r="AO3">
         <v>6.6</v>
       </c>
-      <c r="AM3">
+      <c r="AP3">
         <v>0.16300000000000001</v>
       </c>
-      <c r="AN3">
+      <c r="AQ3">
         <v>12.319000000000001</v>
       </c>
-      <c r="AO3">
+      <c r="AR3">
         <v>0.16800000000000001</v>
       </c>
-      <c r="AP3">
+      <c r="AS3">
         <v>0.30499999999999999</v>
       </c>
-      <c r="AQ3">
+      <c r="AT3">
         <v>200</v>
       </c>
-      <c r="AR3">
+      <c r="AU3">
         <v>10</v>
       </c>
-      <c r="AS3">
+      <c r="AV3">
         <v>90</v>
       </c>
-      <c r="AT3">
+      <c r="AW3">
         <v>100</v>
       </c>
-      <c r="AU3">
+      <c r="AX3">
         <v>2</v>
       </c>
-      <c r="AV3">
+      <c r="AY3">
         <v>0</v>
       </c>
-      <c r="AW3">
+      <c r="AZ3">
         <v>703.62070000000006</v>
       </c>
-      <c r="AX3" s="1">
+      <c r="BA3" s="1">
         <v>579.49980000000005</v>
       </c>
-      <c r="AY3" s="1">
+      <c r="BB3" s="1">
         <v>208.68700000000001</v>
       </c>
-      <c r="AZ3">
+      <c r="BC3">
         <v>78713.626749999996</v>
       </c>
-      <c r="BA3">
+      <c r="BD3">
         <v>793.64156000000003</v>
       </c>
-      <c r="BB3">
+      <c r="BE3">
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1627,103 +1666,112 @@
         <v>7.02</v>
       </c>
       <c r="W4">
+        <v>9.4149999999999991</v>
+      </c>
+      <c r="X4">
+        <v>2.83</v>
+      </c>
+      <c r="Y4">
+        <v>2.214</v>
+      </c>
+      <c r="Z4">
         <v>1E-4</v>
       </c>
-      <c r="X4">
+      <c r="AA4">
         <v>609</v>
       </c>
-      <c r="Y4">
+      <c r="AB4">
         <v>8.1878499999999992</v>
       </c>
-      <c r="Z4">
+      <c r="AC4">
         <v>0.76285499999999995</v>
       </c>
-      <c r="AA4">
+      <c r="AD4">
         <v>0.79295000000000004</v>
       </c>
-      <c r="AB4">
+      <c r="AE4">
         <v>0</v>
       </c>
-      <c r="AC4">
+      <c r="AF4">
         <v>0.5</v>
       </c>
-      <c r="AD4">
+      <c r="AG4">
         <v>0</v>
       </c>
-      <c r="AE4">
+      <c r="AH4">
         <v>0.1</v>
       </c>
-      <c r="AF4">
+      <c r="AI4">
         <v>0.2</v>
       </c>
-      <c r="AG4">
+      <c r="AJ4">
         <v>0.23780499999999999</v>
       </c>
-      <c r="AH4">
+      <c r="AK4">
         <v>0.44724000000000003</v>
       </c>
-      <c r="AI4">
+      <c r="AL4">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AJ4">
+      <c r="AM4">
         <v>2</v>
       </c>
-      <c r="AK4">
+      <c r="AN4">
         <v>-60</v>
       </c>
-      <c r="AL4">
+      <c r="AO4">
         <v>9</v>
       </c>
-      <c r="AM4">
+      <c r="AP4">
         <v>7.8E-2</v>
       </c>
-      <c r="AN4">
+      <c r="AQ4">
         <v>14.824999999999999</v>
       </c>
-      <c r="AO4">
+      <c r="AR4">
         <v>0.108</v>
       </c>
-      <c r="AP4">
+      <c r="AS4">
         <v>0.17710000000000001</v>
-      </c>
-      <c r="AQ4">
-        <v>20</v>
-      </c>
-      <c r="AR4">
-        <v>10</v>
-      </c>
-      <c r="AS4">
-        <v>90</v>
       </c>
       <c r="AT4">
         <v>20</v>
       </c>
       <c r="AU4">
+        <v>10</v>
+      </c>
+      <c r="AV4">
+        <v>90</v>
+      </c>
+      <c r="AW4">
+        <v>20</v>
+      </c>
+      <c r="AX4">
         <v>2</v>
       </c>
-      <c r="AV4">
+      <c r="AY4">
         <v>0.01</v>
       </c>
-      <c r="AW4" s="2">
+      <c r="AZ4" s="2">
         <v>703.62070000000006</v>
       </c>
-      <c r="AX4" s="3">
+      <c r="BA4" s="3">
         <v>579.49980000000005</v>
       </c>
-      <c r="AY4" s="3">
+      <c r="BB4" s="3">
         <v>208.68700000000001</v>
       </c>
-      <c r="AZ4" s="2">
+      <c r="BC4" s="2">
         <v>78713.626749999996</v>
       </c>
-      <c r="BA4" s="2">
+      <c r="BD4" s="2">
         <v>793.64156000000003</v>
       </c>
-      <c r="BB4" s="2">
+      <c r="BE4" s="2">
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1791,103 +1839,112 @@
         <v>7.02</v>
       </c>
       <c r="W5">
+        <v>10.827</v>
+      </c>
+      <c r="X5">
+        <v>3.5430000000000001</v>
+      </c>
+      <c r="Y5">
+        <v>2.3809999999999998</v>
+      </c>
+      <c r="Z5">
         <v>1E-4</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>250</v>
       </c>
-      <c r="Y5">
+      <c r="AB5">
         <v>8.1878499999999992</v>
       </c>
-      <c r="Z5">
+      <c r="AC5">
         <v>0.76285499999999995</v>
       </c>
-      <c r="AA5">
+      <c r="AD5">
         <v>0.79295000000000004</v>
       </c>
-      <c r="AB5">
+      <c r="AE5">
         <v>0</v>
       </c>
-      <c r="AC5">
+      <c r="AF5">
         <v>0.5</v>
       </c>
-      <c r="AD5">
+      <c r="AG5">
         <v>0</v>
       </c>
-      <c r="AE5">
+      <c r="AH5">
         <v>0.1</v>
       </c>
-      <c r="AF5">
+      <c r="AI5">
         <v>0.2</v>
       </c>
-      <c r="AG5">
+      <c r="AJ5">
         <v>0.1</v>
       </c>
-      <c r="AH5">
+      <c r="AK5">
         <v>0.44724000000000003</v>
       </c>
-      <c r="AI5">
+      <c r="AL5">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AJ5">
+      <c r="AM5">
         <v>1</v>
       </c>
-      <c r="AK5">
+      <c r="AN5">
         <v>-33</v>
       </c>
-      <c r="AL5">
+      <c r="AO5">
         <v>6.6</v>
       </c>
-      <c r="AM5">
+      <c r="AP5">
         <v>0.16300000000000001</v>
       </c>
-      <c r="AN5">
+      <c r="AQ5">
         <v>12.319000000000001</v>
       </c>
-      <c r="AO5">
+      <c r="AR5">
         <v>0.16800000000000001</v>
       </c>
-      <c r="AP5">
+      <c r="AS5">
         <v>0.30499999999999999</v>
-      </c>
-      <c r="AQ5">
-        <v>200</v>
-      </c>
-      <c r="AR5">
-        <v>10</v>
-      </c>
-      <c r="AS5">
-        <v>50</v>
       </c>
       <c r="AT5">
         <v>200</v>
       </c>
       <c r="AU5">
+        <v>10</v>
+      </c>
+      <c r="AV5">
+        <v>50</v>
+      </c>
+      <c r="AW5">
+        <v>200</v>
+      </c>
+      <c r="AX5">
         <v>1.5</v>
       </c>
-      <c r="AV5">
+      <c r="AY5">
         <v>0</v>
       </c>
-      <c r="AW5">
+      <c r="AZ5">
         <v>703.62070000000006</v>
       </c>
-      <c r="AX5" s="1">
+      <c r="BA5" s="1">
         <v>579.49980000000005</v>
       </c>
-      <c r="AY5" s="1">
+      <c r="BB5" s="1">
         <v>208.68700000000001</v>
       </c>
-      <c r="AZ5">
+      <c r="BC5">
         <v>78713.626749999996</v>
       </c>
-      <c r="BA5">
+      <c r="BD5">
         <v>793.64156000000003</v>
       </c>
-      <c r="BB5">
+      <c r="BE5">
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1955,127 +2012,136 @@
         <v>7.02</v>
       </c>
       <c r="W6">
+        <v>28.719000000000001</v>
+      </c>
+      <c r="X6">
+        <v>10.939</v>
+      </c>
+      <c r="Y6">
+        <v>4.9160000000000004</v>
+      </c>
+      <c r="Z6">
         <v>1E-4</v>
       </c>
-      <c r="X6">
+      <c r="AA6">
         <v>250</v>
       </c>
-      <c r="Y6">
+      <c r="AB6">
         <v>8.1878499999999992</v>
       </c>
-      <c r="Z6">
+      <c r="AC6">
         <v>0.76285499999999995</v>
       </c>
-      <c r="AA6">
+      <c r="AD6">
         <v>0.79295000000000004</v>
       </c>
-      <c r="AB6">
+      <c r="AE6">
         <v>0</v>
       </c>
-      <c r="AC6">
+      <c r="AF6">
         <v>0.5</v>
       </c>
-      <c r="AD6">
+      <c r="AG6">
         <v>0</v>
       </c>
-      <c r="AE6">
+      <c r="AH6">
         <v>0.1</v>
       </c>
-      <c r="AF6">
+      <c r="AI6">
         <v>0.2</v>
       </c>
-      <c r="AG6">
+      <c r="AJ6">
         <v>0.1</v>
       </c>
-      <c r="AH6">
+      <c r="AK6">
         <v>0.44724000000000003</v>
       </c>
-      <c r="AI6">
+      <c r="AL6">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AJ6">
+      <c r="AM6">
         <v>1</v>
       </c>
-      <c r="AK6">
+      <c r="AN6">
         <v>-33</v>
       </c>
-      <c r="AL6">
+      <c r="AO6">
         <v>6.6</v>
       </c>
-      <c r="AM6">
+      <c r="AP6">
         <v>0.16300000000000001</v>
       </c>
-      <c r="AN6">
+      <c r="AQ6">
         <v>12.319000000000001</v>
       </c>
-      <c r="AO6">
+      <c r="AR6">
         <v>0.16800000000000001</v>
       </c>
-      <c r="AP6">
+      <c r="AS6">
         <v>0.30499999999999999</v>
-      </c>
-      <c r="AQ6">
-        <v>100</v>
-      </c>
-      <c r="AR6">
-        <v>10</v>
-      </c>
-      <c r="AS6">
-        <v>20</v>
       </c>
       <c r="AT6">
         <v>100</v>
       </c>
       <c r="AU6">
+        <v>10</v>
+      </c>
+      <c r="AV6">
+        <v>20</v>
+      </c>
+      <c r="AW6">
+        <v>100</v>
+      </c>
+      <c r="AX6">
         <v>3</v>
       </c>
-      <c r="AV6">
+      <c r="AY6">
         <v>0</v>
       </c>
-      <c r="AW6">
+      <c r="AZ6">
         <v>703.62070000000006</v>
       </c>
-      <c r="AX6" s="1">
+      <c r="BA6" s="1">
         <v>579.49980000000005</v>
       </c>
-      <c r="AY6" s="1">
+      <c r="BB6" s="1">
         <v>208.68700000000001</v>
       </c>
-      <c r="AZ6">
+      <c r="BC6">
         <v>78713.626749999996</v>
       </c>
-      <c r="BA6">
+      <c r="BD6">
         <v>793.64156000000003</v>
       </c>
-      <c r="BB6">
+      <c r="BE6">
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="59" spans="39:43" x14ac:dyDescent="0.3">
-      <c r="AO59" s="2"/>
+    <row r="59" spans="42:46" x14ac:dyDescent="0.25">
+      <c r="AR59" s="2"/>
     </row>
-    <row r="60" spans="39:43" x14ac:dyDescent="0.3">
-      <c r="AM60" s="1"/>
-      <c r="AN60" s="1"/>
-      <c r="AO60" s="3"/>
+    <row r="60" spans="42:46" x14ac:dyDescent="0.25">
       <c r="AP60" s="1"/>
       <c r="AQ60" s="1"/>
+      <c r="AR60" s="3"/>
+      <c r="AS60" s="1"/>
+      <c r="AT60" s="1"/>
     </row>
-    <row r="61" spans="39:43" x14ac:dyDescent="0.3">
-      <c r="AM61" s="1"/>
-      <c r="AN61" s="1"/>
-      <c r="AO61" s="3"/>
+    <row r="61" spans="42:46" x14ac:dyDescent="0.25">
       <c r="AP61" s="1"/>
       <c r="AQ61" s="1"/>
+      <c r="AR61" s="3"/>
+      <c r="AS61" s="1"/>
+      <c r="AT61" s="1"/>
     </row>
-    <row r="62" spans="39:43" x14ac:dyDescent="0.3">
-      <c r="AO62" s="2"/>
+    <row r="62" spans="42:46" x14ac:dyDescent="0.25">
+      <c r="AR62" s="2"/>
     </row>
-    <row r="63" spans="39:43" x14ac:dyDescent="0.3">
-      <c r="AO63" s="2"/>
+    <row r="63" spans="42:46" x14ac:dyDescent="0.25">
+      <c r="AR63" s="2"/>
     </row>
-    <row r="64" spans="39:43" x14ac:dyDescent="0.3">
-      <c r="AO64" s="2"/>
+    <row r="64" spans="42:46" x14ac:dyDescent="0.25">
+      <c r="AR64" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
settings set for Spasskaya Pad
</commit_message>
<xml_diff>
--- a/specieslist.xlsx
+++ b/specieslist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StefanKruseData\Programmierung\Species\LAVESI_multiplespecies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dmawi\potsdam\data\legacy\Model\Modelling\LAVESI_multiplespecies\LAVESI_multiplespecies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>number</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>heightlogc</t>
+  </si>
+  <si>
+    <t>mwindthrow</t>
   </si>
 </sst>
 </file>
@@ -1017,13 +1020,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE64"/>
+  <dimension ref="A1:BF6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
+      <selection pane="bottomRight" activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,24 +1065,25 @@
     <col min="33" max="33" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.140625" customWidth="1"/>
-    <col min="48" max="48" width="14.85546875" customWidth="1"/>
-    <col min="49" max="49" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.28515625" customWidth="1"/>
+    <col min="37" max="37" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.140625" customWidth="1"/>
+    <col min="49" max="49" width="14.85546875" customWidth="1"/>
+    <col min="50" max="50" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1186,73 +1190,76 @@
         <v>30</v>
       </c>
       <c r="AJ1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>40</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>47</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>52</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>48</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>51</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>53</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>54</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>55</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>56</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>57</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1275,7 +1282,7 @@
         <v>0.16</v>
       </c>
       <c r="H2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I2">
         <v>0.01</v>
@@ -1347,7 +1354,7 @@
         <v>0.01</v>
       </c>
       <c r="AF2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AG2">
         <v>0</v>
@@ -1359,73 +1366,76 @@
         <v>0.2</v>
       </c>
       <c r="AJ2">
+        <v>0.01</v>
+      </c>
+      <c r="AK2">
         <v>0.23780499999999999</v>
       </c>
-      <c r="AK2">
+      <c r="AL2">
         <v>0.44724000000000003</v>
       </c>
-      <c r="AL2">
+      <c r="AM2">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AM2">
+      <c r="AN2">
         <v>4</v>
       </c>
-      <c r="AN2">
+      <c r="AO2">
         <v>-45</v>
       </c>
-      <c r="AO2">
+      <c r="AP2">
         <v>9</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <v>7.8E-2</v>
       </c>
-      <c r="AQ2">
+      <c r="AR2">
         <v>14.824999999999999</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <v>0.108</v>
       </c>
-      <c r="AS2">
+      <c r="AT2">
         <v>0.17710000000000001</v>
       </c>
-      <c r="AT2">
+      <c r="AU2">
         <v>20</v>
       </c>
-      <c r="AU2">
+      <c r="AV2">
         <v>21.1</v>
       </c>
-      <c r="AV2">
+      <c r="AW2">
         <v>40</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <v>50</v>
       </c>
-      <c r="AX2">
+      <c r="AY2">
         <v>2</v>
       </c>
-      <c r="AY2">
+      <c r="AZ2">
         <v>0.01</v>
       </c>
-      <c r="AZ2">
+      <c r="BA2">
         <v>703.62070000000006</v>
       </c>
-      <c r="BA2" s="1">
+      <c r="BB2" s="1">
         <v>579.49980000000005</v>
       </c>
-      <c r="BB2" s="1">
+      <c r="BC2" s="1">
         <v>208.68700000000001</v>
       </c>
-      <c r="BC2">
+      <c r="BD2">
         <v>78713.626749999996</v>
       </c>
-      <c r="BD2">
+      <c r="BE2">
         <v>793.64156000000003</v>
       </c>
-      <c r="BE2">
+      <c r="BF2">
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1532,73 +1542,76 @@
         <v>0.2</v>
       </c>
       <c r="AJ3">
+        <v>0.01</v>
+      </c>
+      <c r="AK3">
         <v>0.23780499999999999</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>0.44724000000000003</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>1</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>-33</v>
       </c>
-      <c r="AO3">
+      <c r="AP3">
         <v>6.6</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <v>0.16300000000000001</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>12.319000000000001</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>0.16800000000000001</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>0.30499999999999999</v>
       </c>
-      <c r="AT3">
+      <c r="AU3">
         <v>200</v>
       </c>
-      <c r="AU3">
+      <c r="AV3">
         <v>10</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <v>90</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>100</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <v>2</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <v>0</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>703.62070000000006</v>
       </c>
-      <c r="BA3" s="1">
+      <c r="BB3" s="1">
         <v>579.49980000000005</v>
       </c>
-      <c r="BB3" s="1">
+      <c r="BC3" s="1">
         <v>208.68700000000001</v>
       </c>
-      <c r="BC3">
+      <c r="BD3">
         <v>78713.626749999996</v>
       </c>
-      <c r="BD3">
+      <c r="BE3">
         <v>793.64156000000003</v>
       </c>
-      <c r="BE3">
+      <c r="BF3">
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1705,73 +1718,76 @@
         <v>0.2</v>
       </c>
       <c r="AJ4">
+        <v>0.01</v>
+      </c>
+      <c r="AK4">
         <v>0.23780499999999999</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>0.44724000000000003</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>2</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>-60</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>9</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>7.8E-2</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>14.824999999999999</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>0.108</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>0.17710000000000001</v>
       </c>
-      <c r="AT4">
+      <c r="AU4">
         <v>20</v>
       </c>
-      <c r="AU4">
+      <c r="AV4">
         <v>10</v>
       </c>
-      <c r="AV4">
+      <c r="AW4">
         <v>90</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <v>20</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <v>2</v>
       </c>
-      <c r="AY4">
+      <c r="AZ4">
         <v>0.01</v>
       </c>
-      <c r="AZ4" s="2">
+      <c r="BA4" s="2">
         <v>703.62070000000006</v>
       </c>
-      <c r="BA4" s="3">
+      <c r="BB4" s="3">
         <v>579.49980000000005</v>
       </c>
-      <c r="BB4" s="3">
+      <c r="BC4" s="3">
         <v>208.68700000000001</v>
       </c>
-      <c r="BC4" s="2">
+      <c r="BD4" s="2">
         <v>78713.626749999996</v>
       </c>
-      <c r="BD4" s="2">
+      <c r="BE4" s="2">
         <v>793.64156000000003</v>
       </c>
-      <c r="BE4" s="2">
+      <c r="BF4" s="2">
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1878,73 +1894,76 @@
         <v>0.2</v>
       </c>
       <c r="AJ5">
+        <v>0.01</v>
+      </c>
+      <c r="AK5">
         <v>0.1</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>0.44724000000000003</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>1</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>-33</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>6.6</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>0.16300000000000001</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>12.319000000000001</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>0.16800000000000001</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>0.30499999999999999</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>200</v>
       </c>
-      <c r="AU5">
+      <c r="AV5">
         <v>10</v>
       </c>
-      <c r="AV5">
+      <c r="AW5">
         <v>50</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <v>200</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>1.5</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>0</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <v>703.62070000000006</v>
       </c>
-      <c r="BA5" s="1">
+      <c r="BB5" s="1">
         <v>579.49980000000005</v>
       </c>
-      <c r="BB5" s="1">
+      <c r="BC5" s="1">
         <v>208.68700000000001</v>
       </c>
-      <c r="BC5">
+      <c r="BD5">
         <v>78713.626749999996</v>
       </c>
-      <c r="BD5">
+      <c r="BE5">
         <v>793.64156000000003</v>
       </c>
-      <c r="BE5">
+      <c r="BF5">
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2051,97 +2070,74 @@
         <v>0.2</v>
       </c>
       <c r="AJ6">
+        <v>0.01</v>
+      </c>
+      <c r="AK6">
         <v>0.1</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>0.44724000000000003</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>1</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>-33</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>6.6</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>0.16300000000000001</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>12.319000000000001</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>0.16800000000000001</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>0.30499999999999999</v>
       </c>
-      <c r="AT6">
+      <c r="AU6">
         <v>100</v>
       </c>
-      <c r="AU6">
+      <c r="AV6">
         <v>10</v>
       </c>
-      <c r="AV6">
+      <c r="AW6">
         <v>20</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <v>100</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>3</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <v>0</v>
       </c>
-      <c r="AZ6">
+      <c r="BA6">
         <v>703.62070000000006</v>
       </c>
-      <c r="BA6" s="1">
+      <c r="BB6" s="1">
         <v>579.49980000000005</v>
       </c>
-      <c r="BB6" s="1">
+      <c r="BC6" s="1">
         <v>208.68700000000001</v>
       </c>
-      <c r="BC6">
+      <c r="BD6">
         <v>78713.626749999996</v>
       </c>
-      <c r="BD6">
+      <c r="BE6">
         <v>793.64156000000003</v>
       </c>
-      <c r="BE6">
+      <c r="BF6">
         <v>73.913020000000003</v>
       </c>
-    </row>
-    <row r="59" spans="42:46" x14ac:dyDescent="0.25">
-      <c r="AR59" s="2"/>
-    </row>
-    <row r="60" spans="42:46" x14ac:dyDescent="0.25">
-      <c r="AP60" s="1"/>
-      <c r="AQ60" s="1"/>
-      <c r="AR60" s="3"/>
-      <c r="AS60" s="1"/>
-      <c r="AT60" s="1"/>
-    </row>
-    <row r="61" spans="42:46" x14ac:dyDescent="0.25">
-      <c r="AP61" s="1"/>
-      <c r="AQ61" s="1"/>
-      <c r="AR61" s="3"/>
-      <c r="AS61" s="1"/>
-      <c r="AT61" s="1"/>
-    </row>
-    <row r="62" spans="42:46" x14ac:dyDescent="0.25">
-      <c r="AR62" s="2"/>
-    </row>
-    <row r="63" spans="42:46" x14ac:dyDescent="0.25">
-      <c r="AR63" s="2"/>
-    </row>
-    <row r="64" spans="42:46" x14ac:dyDescent="0.25">
-      <c r="AR64" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added further up to 5 km areas around Spasskaya Pad; updated species information about Pinus sibirica and Picea obovata
</commit_message>
<xml_diff>
--- a/specieslist.xlsx
+++ b/specieslist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>number</t>
   </si>
@@ -208,14 +208,18 @@
   </si>
   <si>
     <t>mwindthrow</t>
+  </si>
+  <si>
+    <t>PISI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -694,11 +698,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1020,70 +1025,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF6"/>
+  <dimension ref="A1:BF7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD8" sqref="AD8"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.28515625" customWidth="1"/>
-    <col min="37" max="37" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.140625" customWidth="1"/>
-    <col min="49" max="49" width="14.85546875" customWidth="1"/>
-    <col min="50" max="50" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.33203125" customWidth="1"/>
+    <col min="37" max="37" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.109375" customWidth="1"/>
+    <col min="49" max="49" width="14.88671875" customWidth="1"/>
+    <col min="50" max="50" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1290,22 +1296,22 @@
       <c r="J2">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="4">
         <v>-1.331944E-4</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="4">
         <v>1.4706535999999999E-3</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="4">
         <v>-0.80558140430000003</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="4">
         <v>-1.331944E-4</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="4">
         <v>1.4706535999999999E-3</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="4">
         <v>-0.80558140430000003</v>
       </c>
       <c r="Q2">
@@ -1435,7 +1441,7 @@
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>0.16</v>
       </c>
       <c r="H3">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I3">
         <v>0.01</v>
@@ -1466,22 +1472,22 @@
       <c r="J3">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="4">
         <v>-8.9999999999999998E-4</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="4">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="4">
         <v>-1.01</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="4">
         <v>-8.9999999999999998E-4</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="4">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="4">
         <v>-1.01</v>
       </c>
       <c r="Q3">
@@ -1521,16 +1527,16 @@
         <v>8.1878499999999992</v>
       </c>
       <c r="AC3">
-        <v>0.76285499999999995</v>
+        <v>0.4</v>
       </c>
       <c r="AD3">
         <v>0.79295000000000004</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AF3">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AG3">
         <v>0</v>
@@ -1551,7 +1557,7 @@
         <v>0.44724000000000003</v>
       </c>
       <c r="AM3">
-        <v>0.55803000000000003</v>
+        <v>0.999</v>
       </c>
       <c r="AN3">
         <v>1</v>
@@ -1578,10 +1584,10 @@
         <v>200</v>
       </c>
       <c r="AV3">
-        <v>10</v>
+        <v>21.1</v>
       </c>
       <c r="AW3">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="AX3">
         <v>100</v>
@@ -1611,7 +1617,7 @@
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1634,7 +1640,7 @@
         <v>0.16</v>
       </c>
       <c r="H4">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I4">
         <v>0.01</v>
@@ -1642,22 +1648,22 @@
       <c r="J4">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="4">
         <v>0.03</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="4">
         <v>-1.98</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="4">
         <v>0.03</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="4">
         <v>-1.98</v>
       </c>
       <c r="Q4">
@@ -1697,16 +1703,16 @@
         <v>8.1878499999999992</v>
       </c>
       <c r="AC4">
-        <v>0.76285499999999995</v>
+        <v>0.4</v>
       </c>
       <c r="AD4">
         <v>0.79295000000000004</v>
       </c>
       <c r="AE4">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AF4">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AG4">
         <v>0</v>
@@ -1754,10 +1760,10 @@
         <v>20</v>
       </c>
       <c r="AV4">
-        <v>10</v>
+        <v>21.1</v>
       </c>
       <c r="AW4">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="AX4">
         <v>20</v>
@@ -1787,7 +1793,7 @@
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>0.63931000000000004</v>
+        <v>0.9</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -1810,7 +1816,7 @@
         <v>0.16</v>
       </c>
       <c r="H5">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I5">
         <v>0.01</v>
@@ -1818,23 +1824,23 @@
       <c r="J5">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K5">
-        <v>-8.9999999999999998E-4</v>
-      </c>
-      <c r="L5">
-        <v>5.5999999999999999E-3</v>
-      </c>
-      <c r="M5">
-        <v>-1.01</v>
-      </c>
-      <c r="N5">
-        <v>-8.9999999999999998E-4</v>
-      </c>
-      <c r="O5">
-        <v>5.5999999999999999E-3</v>
-      </c>
-      <c r="P5">
-        <v>-1.01</v>
+      <c r="K5" s="4">
+        <v>-2.5293869999999999E-4</v>
+      </c>
+      <c r="L5" s="4">
+        <v>6.5782078999999999E-3</v>
+      </c>
+      <c r="M5" s="4">
+        <v>-1.3198466818000001</v>
+      </c>
+      <c r="N5" s="4">
+        <v>-2.5293869999999999E-4</v>
+      </c>
+      <c r="O5" s="4">
+        <v>6.5782078999999999E-3</v>
+      </c>
+      <c r="P5" s="4">
+        <v>-1.3198466818000001</v>
       </c>
       <c r="Q5">
         <v>42.88</v>
@@ -1873,16 +1879,16 @@
         <v>8.1878499999999992</v>
       </c>
       <c r="AC5">
-        <v>0.76285499999999995</v>
+        <v>0.4</v>
       </c>
       <c r="AD5">
         <v>0.79295000000000004</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AF5">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AG5">
         <v>0</v>
@@ -1897,13 +1903,13 @@
         <v>0.01</v>
       </c>
       <c r="AK5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="AL5">
         <v>0.44724000000000003</v>
       </c>
       <c r="AM5">
-        <v>0.55803000000000003</v>
+        <v>0.999</v>
       </c>
       <c r="AN5">
         <v>1</v>
@@ -1930,10 +1936,10 @@
         <v>200</v>
       </c>
       <c r="AV5">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="AW5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AX5">
         <v>200</v>
@@ -1963,7 +1969,7 @@
         <v>73.913020000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1974,7 +1980,7 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>0.63931000000000004</v>
+        <v>0.95</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -1986,7 +1992,7 @@
         <v>0.16</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I6">
         <v>0.01</v>
@@ -1994,23 +2000,23 @@
       <c r="J6">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K6">
-        <v>-8.9999999999999998E-4</v>
-      </c>
-      <c r="L6">
-        <v>5.5999999999999999E-3</v>
-      </c>
-      <c r="M6">
-        <v>-1.01</v>
-      </c>
-      <c r="N6">
-        <v>-8.9999999999999998E-4</v>
-      </c>
-      <c r="O6">
-        <v>5.5999999999999999E-3</v>
-      </c>
-      <c r="P6">
-        <v>-1.01</v>
+      <c r="K6" s="4">
+        <v>-2.5293869999999999E-4</v>
+      </c>
+      <c r="L6" s="4">
+        <v>6.5782078999999999E-3</v>
+      </c>
+      <c r="M6" s="4">
+        <v>-1.3198466818000001</v>
+      </c>
+      <c r="N6" s="4">
+        <v>-2.5293869999999999E-4</v>
+      </c>
+      <c r="O6" s="4">
+        <v>6.5782078999999999E-3</v>
+      </c>
+      <c r="P6" s="4">
+        <v>-1.3198466818000001</v>
       </c>
       <c r="Q6">
         <v>42.88</v>
@@ -2049,16 +2055,16 @@
         <v>8.1878499999999992</v>
       </c>
       <c r="AC6">
-        <v>0.76285499999999995</v>
+        <v>0.4</v>
       </c>
       <c r="AD6">
         <v>0.79295000000000004</v>
       </c>
       <c r="AE6">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AF6">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AG6">
         <v>0</v>
@@ -2073,13 +2079,13 @@
         <v>0.01</v>
       </c>
       <c r="AK6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="AL6">
         <v>0.44724000000000003</v>
       </c>
       <c r="AM6">
-        <v>0.55803000000000003</v>
+        <v>0.999</v>
       </c>
       <c r="AN6">
         <v>1</v>
@@ -2106,10 +2112,10 @@
         <v>100</v>
       </c>
       <c r="AV6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AW6">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="AX6">
         <v>100</v>
@@ -2136,6 +2142,182 @@
         <v>793.64156000000003</v>
       </c>
       <c r="BF6">
+        <v>73.913020000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>0.95</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>2.4</v>
+      </c>
+      <c r="G7">
+        <v>0.16</v>
+      </c>
+      <c r="H7">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>0.01</v>
+      </c>
+      <c r="J7">
+        <v>0.44797500000000001</v>
+      </c>
+      <c r="K7" s="4">
+        <v>-2.5293869999999999E-4</v>
+      </c>
+      <c r="L7" s="4">
+        <v>6.5782078999999999E-3</v>
+      </c>
+      <c r="M7" s="4">
+        <v>-1.3198466818000001</v>
+      </c>
+      <c r="N7" s="4">
+        <v>-2.5293869999999999E-4</v>
+      </c>
+      <c r="O7" s="4">
+        <v>6.5782078999999999E-3</v>
+      </c>
+      <c r="P7" s="4">
+        <v>-1.3198466818000001</v>
+      </c>
+      <c r="Q7">
+        <v>42.88</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>42.88</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>44.431629999999998</v>
+      </c>
+      <c r="V7">
+        <v>7.02</v>
+      </c>
+      <c r="W7">
+        <v>11.590869</v>
+      </c>
+      <c r="X7">
+        <v>4.1021150000000004</v>
+      </c>
+      <c r="Y7">
+        <v>3.057776</v>
+      </c>
+      <c r="Z7">
+        <v>1E-4</v>
+      </c>
+      <c r="AA7">
+        <v>250</v>
+      </c>
+      <c r="AB7">
+        <v>8.1878499999999992</v>
+      </c>
+      <c r="AC7">
+        <v>0.4</v>
+      </c>
+      <c r="AD7">
+        <v>0.79295000000000004</v>
+      </c>
+      <c r="AE7">
+        <v>0.01</v>
+      </c>
+      <c r="AF7">
+        <v>0.2</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0.1</v>
+      </c>
+      <c r="AI7">
+        <v>0.2</v>
+      </c>
+      <c r="AJ7">
+        <v>0.01</v>
+      </c>
+      <c r="AK7">
+        <v>0.5</v>
+      </c>
+      <c r="AL7">
+        <v>0.44724000000000003</v>
+      </c>
+      <c r="AM7">
+        <v>0.999</v>
+      </c>
+      <c r="AN7">
+        <v>1</v>
+      </c>
+      <c r="AO7">
+        <v>-33</v>
+      </c>
+      <c r="AP7">
+        <v>6.6</v>
+      </c>
+      <c r="AQ7">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="AR7">
+        <v>12.319000000000001</v>
+      </c>
+      <c r="AS7">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AT7">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="AU7">
+        <v>200</v>
+      </c>
+      <c r="AV7">
+        <v>21.1</v>
+      </c>
+      <c r="AW7">
+        <v>40</v>
+      </c>
+      <c r="AX7">
+        <v>100</v>
+      </c>
+      <c r="AY7">
+        <v>3</v>
+      </c>
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BA7">
+        <v>703.62070000000006</v>
+      </c>
+      <c r="BB7" s="1">
+        <v>579.49980000000005</v>
+      </c>
+      <c r="BC7" s="1">
+        <v>208.68700000000001</v>
+      </c>
+      <c r="BD7">
+        <v>78713.626749999996</v>
+      </c>
+      <c r="BE7">
+        <v>793.64156000000003</v>
+      </c>
+      <c r="BF7">
         <v>73.913020000000003</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final commit for scenario simulations
</commit_message>
<xml_diff>
--- a/specieslist.xlsx
+++ b/specieslist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dmawi\potsdam\data\legacy\Model\Modelling\LAVESI_multiplespecies\LAVESI_multiplespecies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dmawi\potsdam\data\legacy\Model\Modelling\CryogridLAVESI\CouplingMaster\LAVESI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>number</t>
   </si>
@@ -211,15 +211,28 @@
   </si>
   <si>
     <t>PISI</t>
+  </si>
+  <si>
+    <t>deciduous</t>
+  </si>
+  <si>
+    <t>crownradiusestslope</t>
+  </si>
+  <si>
+    <t>crownradiusestinterc</t>
+  </si>
+  <si>
+    <t>leafareaslope</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -698,12 +711,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="6" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="6" fillId="2" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1025,71 +1042,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF7"/>
+  <dimension ref="A1:BJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="23.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.33203125" customWidth="1"/>
-    <col min="37" max="37" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.109375" customWidth="1"/>
-    <col min="49" max="49" width="14.88671875" customWidth="1"/>
-    <col min="50" max="50" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.28515625" customWidth="1"/>
+    <col min="37" max="37" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.140625" customWidth="1"/>
+    <col min="49" max="49" width="14.85546875" customWidth="1"/>
+    <col min="50" max="50" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1264,24 +1281,36 @@
       <c r="BF1" t="s">
         <v>58</v>
       </c>
+      <c r="BG1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0.63931000000000004</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>60.1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>0.86</v>
       </c>
       <c r="G2">
@@ -1296,22 +1325,22 @@
       <c r="J2">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="7">
         <v>-1.331944E-4</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="7">
         <v>1.4706535999999999E-3</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="7">
         <v>-0.80558140430000003</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <v>-1.331944E-4</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="3">
         <v>1.4706535999999999E-3</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="3">
         <v>-0.80558140430000003</v>
       </c>
       <c r="Q2">
@@ -1332,13 +1361,13 @@
       <c r="V2">
         <v>7.02</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="6">
         <v>9.4149999999999991</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="6">
         <v>2.83</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="6">
         <v>2.214</v>
       </c>
       <c r="Z2">
@@ -1383,7 +1412,7 @@
       <c r="AM2">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AN2">
+      <c r="AN2" s="1">
         <v>4</v>
       </c>
       <c r="AO2">
@@ -1404,60 +1433,72 @@
       <c r="AT2">
         <v>0.17710000000000001</v>
       </c>
-      <c r="AU2">
+      <c r="AU2" s="1">
         <v>20</v>
       </c>
-      <c r="AV2">
+      <c r="AV2" s="1">
         <v>21.1</v>
       </c>
-      <c r="AW2">
+      <c r="AW2" s="1">
         <v>40</v>
       </c>
-      <c r="AX2">
+      <c r="AX2" s="1">
         <v>50</v>
       </c>
-      <c r="AY2">
+      <c r="AY2" s="6">
         <v>2</v>
       </c>
-      <c r="AZ2">
+      <c r="AZ2" s="6">
         <v>0.01</v>
       </c>
-      <c r="BA2">
+      <c r="BA2" s="6">
         <v>703.62070000000006</v>
       </c>
-      <c r="BB2" s="1">
+      <c r="BB2" s="8">
         <v>579.49980000000005</v>
       </c>
-      <c r="BC2" s="1">
+      <c r="BC2" s="8">
         <v>208.68700000000001</v>
       </c>
-      <c r="BD2">
+      <c r="BD2" s="6">
         <v>78713.626749999996</v>
       </c>
-      <c r="BE2">
+      <c r="BE2" s="6">
         <v>793.64156000000003</v>
       </c>
-      <c r="BF2">
+      <c r="BF2" s="6">
         <v>73.913020000000003</v>
       </c>
+      <c r="BG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH2" s="4">
+        <v>1.067957</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>2.0632130000000002</v>
+      </c>
+      <c r="BJ2" s="1">
+        <v>13.744300000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0.63931000000000004</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>45</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>0.93</v>
       </c>
       <c r="G3">
@@ -1472,22 +1513,22 @@
       <c r="J3">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="7">
         <v>-8.9999999999999998E-4</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="7">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="7">
         <v>-1.01</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>-8.9999999999999998E-4</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="3">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="3">
         <v>-1.01</v>
       </c>
       <c r="Q3">
@@ -1508,13 +1549,13 @@
       <c r="V3">
         <v>7.02</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="6">
         <v>9.4149999999999991</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="6">
         <v>2.83</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="6">
         <v>2.214</v>
       </c>
       <c r="Z3">
@@ -1559,7 +1600,7 @@
       <c r="AM3">
         <v>0.999</v>
       </c>
-      <c r="AN3">
+      <c r="AN3" s="1">
         <v>1</v>
       </c>
       <c r="AO3">
@@ -1580,60 +1621,73 @@
       <c r="AT3">
         <v>0.30499999999999999</v>
       </c>
-      <c r="AU3">
+      <c r="AU3" s="1">
         <v>200</v>
       </c>
-      <c r="AV3">
-        <v>21.1</v>
-      </c>
-      <c r="AW3">
+      <c r="AV3" s="1">
+        <f>21.1-0.1*21.1</f>
+        <v>18.990000000000002</v>
+      </c>
+      <c r="AW3" s="1">
         <v>40</v>
       </c>
-      <c r="AX3">
+      <c r="AX3" s="6">
         <v>100</v>
       </c>
-      <c r="AY3">
+      <c r="AY3" s="6">
         <v>2</v>
       </c>
-      <c r="AZ3">
+      <c r="AZ3" s="6">
         <v>0</v>
       </c>
-      <c r="BA3">
+      <c r="BA3" s="6">
         <v>703.62070000000006</v>
       </c>
-      <c r="BB3" s="1">
+      <c r="BB3" s="8">
         <v>579.49980000000005</v>
       </c>
-      <c r="BC3" s="1">
+      <c r="BC3" s="8">
         <v>208.68700000000001</v>
       </c>
-      <c r="BD3">
+      <c r="BD3" s="6">
         <v>78713.626749999996</v>
       </c>
-      <c r="BE3">
+      <c r="BE3" s="6">
         <v>793.64156000000003</v>
       </c>
-      <c r="BF3">
+      <c r="BF3" s="6">
         <v>73.913020000000003</v>
       </c>
+      <c r="BG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH3" s="5">
+        <v>1.067957</v>
+      </c>
+      <c r="BI3" s="6">
+        <v>2.0632130000000002</v>
+      </c>
+      <c r="BJ3" s="6">
+        <v>13.744300000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>0.63931000000000004</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>60.1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>0.86</v>
       </c>
       <c r="G4">
@@ -1648,22 +1702,22 @@
       <c r="J4">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="7">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="7">
         <v>0.03</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="7">
         <v>-1.98</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <v>0.03</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <v>-1.98</v>
       </c>
       <c r="Q4">
@@ -1684,20 +1738,20 @@
       <c r="V4">
         <v>7.02</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="6">
         <v>9.4149999999999991</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="6">
         <v>2.83</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="6">
         <v>2.214</v>
       </c>
       <c r="Z4">
         <v>1E-4</v>
       </c>
       <c r="AA4">
-        <v>609</v>
+        <v>500</v>
       </c>
       <c r="AB4">
         <v>8.1878499999999992</v>
@@ -1735,7 +1789,7 @@
       <c r="AM4">
         <v>0.55803000000000003</v>
       </c>
-      <c r="AN4">
+      <c r="AN4" s="1">
         <v>2</v>
       </c>
       <c r="AO4">
@@ -1756,60 +1810,72 @@
       <c r="AT4">
         <v>0.17710000000000001</v>
       </c>
-      <c r="AU4">
+      <c r="AU4" s="1">
         <v>20</v>
       </c>
-      <c r="AV4">
+      <c r="AV4" s="1">
         <v>21.1</v>
       </c>
-      <c r="AW4">
+      <c r="AW4" s="1">
         <v>40</v>
       </c>
-      <c r="AX4">
+      <c r="AX4" s="6">
         <v>20</v>
       </c>
-      <c r="AY4">
+      <c r="AY4" s="6">
         <v>2</v>
       </c>
-      <c r="AZ4">
+      <c r="AZ4" s="6">
         <v>0.01</v>
       </c>
-      <c r="BA4" s="2">
+      <c r="BA4" s="1">
         <v>703.62070000000006</v>
       </c>
-      <c r="BB4" s="3">
+      <c r="BB4" s="2">
         <v>579.49980000000005</v>
       </c>
-      <c r="BC4" s="3">
+      <c r="BC4" s="2">
         <v>208.68700000000001</v>
       </c>
-      <c r="BD4" s="2">
+      <c r="BD4" s="1">
         <v>78713.626749999996</v>
       </c>
-      <c r="BE4" s="2">
+      <c r="BE4" s="1">
         <v>793.64156000000003</v>
       </c>
-      <c r="BF4" s="2">
+      <c r="BF4" s="1">
         <v>73.913020000000003</v>
       </c>
+      <c r="BG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH4" s="1">
+        <v>0.91933330000000002</v>
+      </c>
+      <c r="BI4" s="1">
+        <v>2.4618495999999999</v>
+      </c>
+      <c r="BJ4" s="1">
+        <v>23.995830000000002</v>
+      </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>0.9</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>15</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>1.2</v>
       </c>
       <c r="G5">
@@ -1824,22 +1890,22 @@
       <c r="J5">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="7">
         <v>-2.5293869999999999E-4</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="7">
         <v>6.5782078999999999E-3</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="7">
         <v>-1.3198466818000001</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>-2.5293869999999999E-4</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="3">
         <v>6.5782078999999999E-3</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="3">
         <v>-1.3198466818000001</v>
       </c>
       <c r="Q5">
@@ -1860,13 +1926,13 @@
       <c r="V5">
         <v>7.02</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="1">
         <v>10.827</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="1">
         <v>3.5430000000000001</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="1">
         <v>2.3809999999999998</v>
       </c>
       <c r="Z5">
@@ -1911,7 +1977,7 @@
       <c r="AM5">
         <v>0.999</v>
       </c>
-      <c r="AN5">
+      <c r="AN5" s="1">
         <v>1</v>
       </c>
       <c r="AO5">
@@ -1932,60 +1998,72 @@
       <c r="AT5">
         <v>0.30499999999999999</v>
       </c>
-      <c r="AU5">
+      <c r="AU5" s="1">
         <v>200</v>
       </c>
-      <c r="AV5">
+      <c r="AV5" s="1">
         <v>25</v>
       </c>
-      <c r="AW5">
+      <c r="AW5" s="1">
         <v>40</v>
       </c>
-      <c r="AX5">
+      <c r="AX5" s="6">
         <v>200</v>
       </c>
-      <c r="AY5">
+      <c r="AY5" s="6">
         <v>1.5</v>
       </c>
-      <c r="AZ5">
+      <c r="AZ5" s="6">
         <v>0</v>
       </c>
-      <c r="BA5">
+      <c r="BA5" s="6">
         <v>703.62070000000006</v>
       </c>
-      <c r="BB5" s="1">
+      <c r="BB5" s="8">
         <v>579.49980000000005</v>
       </c>
-      <c r="BC5" s="1">
+      <c r="BC5" s="8">
         <v>208.68700000000001</v>
       </c>
-      <c r="BD5">
+      <c r="BD5" s="6">
         <v>78713.626749999996</v>
       </c>
-      <c r="BE5">
+      <c r="BE5" s="6">
         <v>793.64156000000003</v>
       </c>
-      <c r="BF5">
+      <c r="BF5" s="6">
         <v>73.913020000000003</v>
       </c>
+      <c r="BG5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="5">
+        <v>1.067957</v>
+      </c>
+      <c r="BI5" s="6">
+        <v>2.0632130000000002</v>
+      </c>
+      <c r="BJ5" s="6">
+        <v>13.744300000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>15</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0.95</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>30</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>2.4</v>
       </c>
       <c r="G6">
@@ -2000,22 +2078,22 @@
       <c r="J6">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="7">
         <v>-2.5293869999999999E-4</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="7">
         <v>6.5782078999999999E-3</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="7">
         <v>-1.3198466818000001</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>-2.5293869999999999E-4</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="3">
         <v>6.5782078999999999E-3</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="3">
         <v>-1.3198466818000001</v>
       </c>
       <c r="Q6">
@@ -2036,13 +2114,13 @@
       <c r="V6">
         <v>7.02</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="1">
         <v>28.719000000000001</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="1">
         <v>10.939</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="1">
         <v>4.9160000000000004</v>
       </c>
       <c r="Z6">
@@ -2087,7 +2165,7 @@
       <c r="AM6">
         <v>0.999</v>
       </c>
-      <c r="AN6">
+      <c r="AN6" s="1">
         <v>1</v>
       </c>
       <c r="AO6">
@@ -2108,60 +2186,72 @@
       <c r="AT6">
         <v>0.30499999999999999</v>
       </c>
-      <c r="AU6">
+      <c r="AU6" s="1">
         <v>100</v>
       </c>
-      <c r="AV6">
+      <c r="AV6" s="1">
         <v>15</v>
       </c>
-      <c r="AW6">
+      <c r="AW6" s="1">
         <v>30</v>
       </c>
-      <c r="AX6">
+      <c r="AX6" s="6">
         <v>100</v>
       </c>
-      <c r="AY6">
+      <c r="AY6" s="6">
         <v>3</v>
       </c>
-      <c r="AZ6">
+      <c r="AZ6" s="6">
         <v>0</v>
       </c>
-      <c r="BA6">
+      <c r="BA6" s="6">
         <v>703.62070000000006</v>
       </c>
-      <c r="BB6" s="1">
+      <c r="BB6" s="8">
         <v>579.49980000000005</v>
       </c>
-      <c r="BC6" s="1">
+      <c r="BC6" s="8">
         <v>208.68700000000001</v>
       </c>
-      <c r="BD6">
+      <c r="BD6" s="6">
         <v>78713.626749999996</v>
       </c>
-      <c r="BE6">
+      <c r="BE6" s="6">
         <v>793.64156000000003</v>
       </c>
-      <c r="BF6">
+      <c r="BF6" s="6">
         <v>73.913020000000003</v>
       </c>
+      <c r="BG6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="5">
+        <v>1.067957</v>
+      </c>
+      <c r="BI6" s="6">
+        <v>2.0632130000000002</v>
+      </c>
+      <c r="BJ6" s="6">
+        <v>13.744300000000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>63</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>15</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>0.95</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>30</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>2.4</v>
       </c>
       <c r="G7">
@@ -2176,22 +2266,22 @@
       <c r="J7">
         <v>0.44797500000000001</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="7">
         <v>-2.5293869999999999E-4</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="7">
         <v>6.5782078999999999E-3</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="7">
         <v>-1.3198466818000001</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <v>-2.5293869999999999E-4</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>6.5782078999999999E-3</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <v>-1.3198466818000001</v>
       </c>
       <c r="Q7">
@@ -2212,13 +2302,13 @@
       <c r="V7">
         <v>7.02</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="1">
         <v>11.590869</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="1">
         <v>4.1021150000000004</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="1">
         <v>3.057776</v>
       </c>
       <c r="Z7">
@@ -2263,7 +2353,7 @@
       <c r="AM7">
         <v>0.999</v>
       </c>
-      <c r="AN7">
+      <c r="AN7" s="1">
         <v>1</v>
       </c>
       <c r="AO7">
@@ -2284,41 +2374,53 @@
       <c r="AT7">
         <v>0.30499999999999999</v>
       </c>
-      <c r="AU7">
+      <c r="AU7" s="1">
         <v>200</v>
       </c>
-      <c r="AV7">
-        <v>21.1</v>
-      </c>
-      <c r="AW7">
+      <c r="AV7" s="1">
+        <v>25</v>
+      </c>
+      <c r="AW7" s="1">
         <v>40</v>
       </c>
-      <c r="AX7">
+      <c r="AX7" s="6">
         <v>100</v>
       </c>
-      <c r="AY7">
+      <c r="AY7" s="6">
         <v>3</v>
       </c>
-      <c r="AZ7">
+      <c r="AZ7" s="6">
         <v>0</v>
       </c>
-      <c r="BA7">
+      <c r="BA7" s="6">
         <v>703.62070000000006</v>
       </c>
-      <c r="BB7" s="1">
+      <c r="BB7" s="8">
         <v>579.49980000000005</v>
       </c>
-      <c r="BC7" s="1">
+      <c r="BC7" s="8">
         <v>208.68700000000001</v>
       </c>
-      <c r="BD7">
+      <c r="BD7" s="6">
         <v>78713.626749999996</v>
       </c>
-      <c r="BE7">
+      <c r="BE7" s="6">
         <v>793.64156000000003</v>
       </c>
-      <c r="BF7">
+      <c r="BF7" s="6">
         <v>73.913020000000003</v>
+      </c>
+      <c r="BG7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="5">
+        <v>1.067957</v>
+      </c>
+      <c r="BI7" s="6">
+        <v>2.0632130000000002</v>
+      </c>
+      <c r="BJ7" s="6">
+        <v>13.744300000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Functional fire module for research simulationsincl. all climate input data
</commit_message>
<xml_diff>
--- a/specieslist.xlsx
+++ b/specieslist.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dmawi\potsdam\data\legacy\Model\Modelling\LAVESI_multiplespecies\LAVESI_multiplespecies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\bioing\user\rglueckler\firesims\LAVESI-multispec\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18B04B2-5B4C-470D-82CF-793F5F38BC91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="specieslist" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>number</t>
   </si>
@@ -211,15 +213,48 @@
   </si>
   <si>
     <t>PISI</t>
+  </si>
+  <si>
+    <t>Testing effect of bark thickness on tree damage</t>
+  </si>
+  <si>
+    <t>tree.firedamage</t>
+  </si>
+  <si>
+    <t>result(firedamage)</t>
+  </si>
+  <si>
+    <t>When bark thickness = 1.5: reduction of 0.05</t>
+  </si>
+  <si>
+    <t>When bark thickness = 3: reduction of 0.1</t>
+  </si>
+  <si>
+    <t>When bark thickness = 2: reduction of 0.066</t>
+  </si>
+  <si>
+    <t>checking treemort vs tree.firedamage</t>
+  </si>
+  <si>
+    <t>treemortality + (((double)tree.firedamage) * (1 / ((double)tree.height / 100) / 150)</t>
+  </si>
+  <si>
+    <t>tree.height</t>
+  </si>
+  <si>
+    <t>result(treemortality)</t>
+  </si>
+  <si>
+    <t>treemortality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -703,7 +738,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="6" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1024,14 +1059,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AS2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2325,4 +2360,230 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FA0CA3-61A9-4056-A2B7-5658C3F92B47}">
+  <dimension ref="A2:K25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="K5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6">
+        <f>C4-(0.1*C5/3)</f>
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>3.333333333333334E-2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="K7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>0.8</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>0.73333333333333339</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>0.5</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>0.1</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1.5</v>
+      </c>
+      <c r="H13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>0.5</v>
+      </c>
+      <c r="G14">
+        <v>1.5</v>
+      </c>
+      <c r="H14">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+      <c r="G15">
+        <v>1.5</v>
+      </c>
+      <c r="H15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25">
+        <f>C22+((C23) * (1/C24/100)/50)</f>
+        <v>0.22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>